<commit_message>
Ajustes en la configuracion
git-svn-id: http://10.34.2.66/svn/sacta-proxy/trunk@19 919647e8-3121-2f49-b100-017848d5475d
</commit_message>
<xml_diff>
--- a/doc/Flujos Sacta.xlsx
+++ b/doc/Flujos Sacta.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Analisis Flujos" sheetId="1" r:id="rId1"/>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="73">
   <si>
     <t>PRX --&gt; SCV</t>
   </si>
@@ -343,6 +343,15 @@
   </si>
   <si>
     <t>IPAPP2:15100 &gt; IPV1:19204</t>
+  </si>
+  <si>
+    <t>IP1</t>
+  </si>
+  <si>
+    <t>APP</t>
+  </si>
+  <si>
+    <t>PRX</t>
   </si>
 </sst>
 </file>
@@ -640,6 +649,533 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="25" name="Grupo 24"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="628650" y="219075"/>
+          <a:ext cx="4257675" cy="2514600"/>
+          <a:chOff x="1828800" y="180975"/>
+          <a:chExt cx="4257675" cy="2514600"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="2" name="Rectángulo 1"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1828800" y="190500"/>
+            <a:ext cx="628650" cy="1171575"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="es-ES" sz="1100"/>
+              <a:t>APP</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="Rectángulo 2"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1828800" y="1524000"/>
+            <a:ext cx="628650" cy="1171575"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="es-ES" sz="1100"/>
+              <a:t>TWR</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="Rectángulo 3"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3657600" y="180975"/>
+            <a:ext cx="609600" cy="2486025"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="es-ES" sz="1100"/>
+              <a:t>PROXY</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="5" name="Rectángulo 4"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5457825" y="828675"/>
+            <a:ext cx="628650" cy="1171575"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="es-ES" sz="1100"/>
+              <a:t>SCV</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="7" name="Conector recto de flecha 6"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="2476500" y="381000"/>
+            <a:ext cx="1209675" cy="9525"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="9" name="Conector recto de flecha 8"/>
+          <xdr:cNvCxnSpPr>
+            <a:endCxn id="2" idx="3"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="2457450" y="771525"/>
+            <a:ext cx="1190625" cy="4763"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="11" name="Conector recto de flecha 10"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="2466975" y="1704975"/>
+            <a:ext cx="1200150" cy="9525"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="13" name="Conector recto de flecha 12"/>
+          <xdr:cNvCxnSpPr>
+            <a:endCxn id="3" idx="3"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="2457450" y="2085975"/>
+            <a:ext cx="1209676" cy="23813"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="16" name="Conector recto de flecha 15"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4267200" y="942975"/>
+            <a:ext cx="1219200" cy="19050"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="20" name="Conector recto de flecha 19"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="5" idx="1"/>
+            <a:endCxn id="4" idx="3"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="4267200" y="1414463"/>
+            <a:ext cx="1190625" cy="9525"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="22" name="CuadroTexto 21"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2762250" y="438150"/>
+            <a:ext cx="689356" cy="264560"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="es-ES" sz="1100"/>
+              <a:t>APP/PRX</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="23" name="CuadroTexto 22"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2733675" y="1781175"/>
+            <a:ext cx="732765" cy="264560"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="es-ES" sz="1100"/>
+              <a:t>TWR/PRX</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="24" name="CuadroTexto 23"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4543425" y="1047750"/>
+            <a:ext cx="681982" cy="264560"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="es-ES" sz="1100"/>
+              <a:t>PRX/SCV</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1460,7 +1996,7 @@
   </sheetPr>
   <dimension ref="B1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -2007,12 +2543,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="J2:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>